<commit_message>
Fixed errors in functional group names in tables
</commit_message>
<xml_diff>
--- a/fuelData/groupDecompositionData/decane.xlsx
+++ b/fuelData/groupDecompositionData/decane.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abinswan/Documents/GroupContributionMethod/Compound_Descriptions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nrel-my.sharepoint.com/personal/dmontgo2_nrel_gov/Documents/Projects/SAF-VTO/GCM/FuelLib/fuelData/groupDecompositionData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0F8E53-401A-404F-B596-15343C8A4942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{FE0F8E53-401A-404F-B596-15343C8A4942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66785648-404E-FB4D-8212-DECE85FFC4C0}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18040" windowHeight="12520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18900" yWindow="5600" windowWidth="18040" windowHeight="12520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -32,240 +32,9 @@
     <t>Compound</t>
   </si>
   <si>
-    <t>CH3 (1)</t>
-  </si>
-  <si>
-    <t>CH2 (2)</t>
-  </si>
-  <si>
-    <t>CH (3)</t>
-  </si>
-  <si>
     <t>C (4)</t>
   </si>
   <si>
-    <t>CH2=CH (1)</t>
-  </si>
-  <si>
-    <t>CH=CH (2)</t>
-  </si>
-  <si>
-    <t>CH2=C (2)</t>
-  </si>
-  <si>
-    <t>CH=C (3)</t>
-  </si>
-  <si>
-    <t>C=C (4)</t>
-  </si>
-  <si>
-    <t>CH2=C=CH(1)</t>
-  </si>
-  <si>
-    <t>ACH (2)</t>
-  </si>
-  <si>
-    <t>AC (3)</t>
-  </si>
-  <si>
-    <t>ACCH3 (2)</t>
-  </si>
-  <si>
-    <t>ACCH2 (3)</t>
-  </si>
-  <si>
-    <t>ACCH (4)</t>
-  </si>
-  <si>
-    <t>OH (1)</t>
-  </si>
-  <si>
-    <t>ACOH (2)</t>
-  </si>
-  <si>
-    <t>CH3CO (1)</t>
-  </si>
-  <si>
-    <t>CH2CO (2)</t>
-  </si>
-  <si>
-    <t>CHO (1)*</t>
-  </si>
-  <si>
-    <t>CH3COO (1)</t>
-  </si>
-  <si>
-    <t>CH2COO (2)</t>
-  </si>
-  <si>
-    <t>HCOO (1)</t>
-  </si>
-  <si>
-    <t>CH30 (1)</t>
-  </si>
-  <si>
-    <t>CH20 (2)</t>
-  </si>
-  <si>
-    <t>CH-O (3)</t>
-  </si>
-  <si>
-    <t>FCH20 (1)*</t>
-  </si>
-  <si>
-    <t>CH2NH2 (1)</t>
-  </si>
-  <si>
-    <t>CHNH2 (2)</t>
-  </si>
-  <si>
-    <t>CH3NH (2)</t>
-  </si>
-  <si>
-    <t>CH2NH (3)</t>
-  </si>
-  <si>
-    <t>CHNH (4)*</t>
-  </si>
-  <si>
-    <t>CH3N (2)</t>
-  </si>
-  <si>
-    <t>CH2N (3)</t>
-  </si>
-  <si>
-    <t>ACNH2 (2)</t>
-  </si>
-  <si>
-    <t>C5H4N (1)</t>
-  </si>
-  <si>
-    <t>C5H3N (2)</t>
-  </si>
-  <si>
-    <t>CH2CN (1)*</t>
-  </si>
-  <si>
-    <t>COOH (1)</t>
-  </si>
-  <si>
-    <t>CH2C1 (1)</t>
-  </si>
-  <si>
-    <t>CHC1 (2)</t>
-  </si>
-  <si>
-    <t>CC1 (3)</t>
-  </si>
-  <si>
-    <t>CHC12 (1)*</t>
-  </si>
-  <si>
-    <t>CC13 (1)</t>
-  </si>
-  <si>
-    <t>CC12 (2)</t>
-  </si>
-  <si>
-    <t>ACC1 (2)</t>
-  </si>
-  <si>
-    <t>CH2N02 (1)*</t>
-  </si>
-  <si>
-    <t>CHN02 (2)*</t>
-  </si>
-  <si>
-    <t>ACN02 (2)*</t>
-  </si>
-  <si>
-    <t>CH2SH (1)</t>
-  </si>
-  <si>
-    <t>C1(1)*</t>
-  </si>
-  <si>
-    <t>Br (1)</t>
-  </si>
-  <si>
-    <t>CH=C (1)</t>
-  </si>
-  <si>
-    <t>C=c (2)*</t>
-  </si>
-  <si>
-    <t>Cl—(C=C) (3)*</t>
-  </si>
-  <si>
-    <t>ACF (2)</t>
-  </si>
-  <si>
-    <t>HCON(CH2)2 (2)*</t>
-  </si>
-  <si>
-    <t>CF3 (1)</t>
-  </si>
-  <si>
-    <t>CF2 (2)</t>
-  </si>
-  <si>
-    <t>CF (3)</t>
-  </si>
-  <si>
-    <t>COO (2)</t>
-  </si>
-  <si>
-    <t>CC12F (1)</t>
-  </si>
-  <si>
-    <t>HCC1F (1)</t>
-  </si>
-  <si>
-    <t>CC1F2 (1)</t>
-  </si>
-  <si>
-    <t>FSpecial (1)</t>
-  </si>
-  <si>
-    <t>CONH2 (1)*</t>
-  </si>
-  <si>
-    <t>CONHCH3 (1)*</t>
-  </si>
-  <si>
-    <t>CONHCH2 (1)*</t>
-  </si>
-  <si>
-    <t>CON(CH3)2 (1)*</t>
-  </si>
-  <si>
-    <t>CONCH2CH2 (3)*</t>
-  </si>
-  <si>
-    <t>CON(CH2)2 (3)*</t>
-  </si>
-  <si>
-    <t>C2H502 (1)*</t>
-  </si>
-  <si>
-    <t>C2H402 (2)</t>
-  </si>
-  <si>
-    <t>CH3S (1)</t>
-  </si>
-  <si>
-    <t>CH2S (2)</t>
-  </si>
-  <si>
-    <t>CHS (3)*</t>
-  </si>
-  <si>
-    <t>C4H3S (1)</t>
-  </si>
-  <si>
-    <t>C4H2S (2)*</t>
-  </si>
-  <si>
     <t>Group j  (CH3)2CH</t>
   </si>
   <si>
@@ -296,106 +65,337 @@
     <t>7 membered ring</t>
   </si>
   <si>
-    <t>CR=CRm—CRp=CRk m, p G (0,1), K n G (0,2)</t>
-  </si>
-  <si>
-    <t>CH3-CHm=CH, m G (0,1), n G (0,2)</t>
-  </si>
-  <si>
-    <t>CH2-CHm=CH, m G (0,1), n G (0,2)</t>
-  </si>
-  <si>
-    <t>CH—CUm=CUn or C—CHm=CH/ m G (0,1), n G (0,2)</t>
-  </si>
-  <si>
     <t>Alicyclic side-chain CcyclicCm m &gt; 1</t>
   </si>
   <si>
-    <t>ch3ch3</t>
-  </si>
-  <si>
-    <t>CHCHO or CCHO*</t>
-  </si>
-  <si>
     <t>CH3COCH2</t>
   </si>
   <si>
     <t>CH3COCH or CH3COC</t>
   </si>
   <si>
-    <t>Ccyclic^=0</t>
-  </si>
-  <si>
-    <t>ACCHO*</t>
-  </si>
-  <si>
-    <t>CHCOOH or CCOOH*</t>
-  </si>
-  <si>
-    <t>ACCOOH*</t>
-  </si>
-  <si>
     <t>CH3COOCH or CH3COOC</t>
   </si>
   <si>
-    <t>COCH2COO or COCHCOO or COCCOO*</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CO—O—CO</t>
-  </si>
-  <si>
-    <t>ACCOO*</t>
-  </si>
-  <si>
     <t>CHOH</t>
   </si>
   <si>
     <t>COH</t>
   </si>
   <si>
-    <t>CHm(OH)CHn(OH)</t>
-  </si>
-  <si>
-    <t>CHm cyclic-OH</t>
-  </si>
-  <si>
-    <t>CHn(OH)CHm(NHp)</t>
-  </si>
-  <si>
-    <t>CHm(NH2)CHn(NH2)*</t>
-  </si>
-  <si>
-    <t>CHm cyclic—NHp—CHn cyclic*</t>
-  </si>
-  <si>
-    <t>CHn_x0003_O_x0003_CHm_x0001_CHp*</t>
-  </si>
-  <si>
-    <t>AC—O—CHm*</t>
-  </si>
-  <si>
-    <t>CHm cyclic—S—CHn cyclic</t>
-  </si>
-  <si>
-    <t>CHn_x0001_CHm—F</t>
-  </si>
-  <si>
-    <t>CHn_x0001_CHm—Br*</t>
-  </si>
-  <si>
-    <t>CHn_x0001_CHm—I*</t>
-  </si>
-  <si>
-    <t>ACBr*</t>
-  </si>
-  <si>
-    <t>ACI*</t>
-  </si>
-  <si>
-    <t>CHm(NH2)—COOH*</t>
-  </si>
-  <si>
     <t>n-C010</t>
+  </si>
+  <si>
+    <t>CH3</t>
+  </si>
+  <si>
+    <t>CH2</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>CH2=CH</t>
+  </si>
+  <si>
+    <t>CH=CH</t>
+  </si>
+  <si>
+    <t>CH2=C</t>
+  </si>
+  <si>
+    <t>CH=C</t>
+  </si>
+  <si>
+    <t>C=C</t>
+  </si>
+  <si>
+    <t>CH2=C=CH</t>
+  </si>
+  <si>
+    <t>ACH</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>ACCH3</t>
+  </si>
+  <si>
+    <t>ACCH2</t>
+  </si>
+  <si>
+    <t>ACCH</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>ACOH</t>
+  </si>
+  <si>
+    <t>CH3CO</t>
+  </si>
+  <si>
+    <t>CH2CO</t>
+  </si>
+  <si>
+    <t>CHO</t>
+  </si>
+  <si>
+    <t>CH3COO</t>
+  </si>
+  <si>
+    <t>CH2COO</t>
+  </si>
+  <si>
+    <t>HCOO</t>
+  </si>
+  <si>
+    <t>CH3O</t>
+  </si>
+  <si>
+    <t>CH2O</t>
+  </si>
+  <si>
+    <t>CH-O</t>
+  </si>
+  <si>
+    <t>FCH2O</t>
+  </si>
+  <si>
+    <t>CH2NH2</t>
+  </si>
+  <si>
+    <t>CHNH2</t>
+  </si>
+  <si>
+    <t>CH3NH</t>
+  </si>
+  <si>
+    <t>CH2NH</t>
+  </si>
+  <si>
+    <t>CHNH</t>
+  </si>
+  <si>
+    <t>CH3N</t>
+  </si>
+  <si>
+    <t>CH2N</t>
+  </si>
+  <si>
+    <t>ACNH2</t>
+  </si>
+  <si>
+    <t>C5H4N</t>
+  </si>
+  <si>
+    <t>C5H3N</t>
+  </si>
+  <si>
+    <t>CH2CN</t>
+  </si>
+  <si>
+    <t>COOH</t>
+  </si>
+  <si>
+    <t>CH2CL</t>
+  </si>
+  <si>
+    <t>CHCL</t>
+  </si>
+  <si>
+    <t>CCL</t>
+  </si>
+  <si>
+    <t>CHCL2</t>
+  </si>
+  <si>
+    <t>CCL2</t>
+  </si>
+  <si>
+    <t>CCL3</t>
+  </si>
+  <si>
+    <t>ACCL</t>
+  </si>
+  <si>
+    <t>CH2NO2</t>
+  </si>
+  <si>
+    <t>CHNO2</t>
+  </si>
+  <si>
+    <t>ACNO2</t>
+  </si>
+  <si>
+    <t>CH2SH</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>CH=-C</t>
+  </si>
+  <si>
+    <t>C=-c</t>
+  </si>
+  <si>
+    <t>CL—(C=C)</t>
+  </si>
+  <si>
+    <t>ACF</t>
+  </si>
+  <si>
+    <t>HCON(CH2)2</t>
+  </si>
+  <si>
+    <t>CF3</t>
+  </si>
+  <si>
+    <t>CF2</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>COO</t>
+  </si>
+  <si>
+    <t>CCL2F</t>
+  </si>
+  <si>
+    <t>HCCLF</t>
+  </si>
+  <si>
+    <t>CCLF2</t>
+  </si>
+  <si>
+    <t>Fspecial</t>
+  </si>
+  <si>
+    <t>CONH2</t>
+  </si>
+  <si>
+    <t>CONHCH3</t>
+  </si>
+  <si>
+    <t>CONHCH2</t>
+  </si>
+  <si>
+    <t>CON(CH3)2</t>
+  </si>
+  <si>
+    <t>CONCH3CH2</t>
+  </si>
+  <si>
+    <t>CON(CH2)2</t>
+  </si>
+  <si>
+    <t>C2H5O2</t>
+  </si>
+  <si>
+    <t>C2H4O2</t>
+  </si>
+  <si>
+    <t>CH3S</t>
+  </si>
+  <si>
+    <t>CH2S</t>
+  </si>
+  <si>
+    <t>CHS</t>
+  </si>
+  <si>
+    <t>C4H3S</t>
+  </si>
+  <si>
+    <t>C4H2S</t>
+  </si>
+  <si>
+    <t>CHn=CHm—CHp=CHk k,n,m,p in (0,2)</t>
+  </si>
+  <si>
+    <t>CH3-CHm=CH, m in (0,1), n in (0,2)</t>
+  </si>
+  <si>
+    <t>CH2-CHm=CHn, m, n in (0,2)</t>
+  </si>
+  <si>
+    <t>CH-CHm=CHn or C-CHm=CHn, m,n m in (0,2)</t>
+  </si>
+  <si>
+    <t>CH3CH3</t>
+  </si>
+  <si>
+    <t>CHCHO or CCHO</t>
+  </si>
+  <si>
+    <t>Ccyclic(=0)</t>
+  </si>
+  <si>
+    <t>ACCHO</t>
+  </si>
+  <si>
+    <t>CHCOOH or CCOOH</t>
+  </si>
+  <si>
+    <t>ACCOOH</t>
+  </si>
+  <si>
+    <t>COCH2COO or COCHCOO or COCCOO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CO-O-CO</t>
+  </si>
+  <si>
+    <t>ACCOO</t>
+  </si>
+  <si>
+    <t>CHm(OH)CHn(OH), m,n in (0,2)</t>
+  </si>
+  <si>
+    <t>CHm cyclic-OH, m in (0,1)</t>
+  </si>
+  <si>
+    <t>CHm(OH)CHn(NHp), m,n,p in (0,3)</t>
+  </si>
+  <si>
+    <t>CHm(NH2)CHn(NH2)</t>
+  </si>
+  <si>
+    <t>CHm cyclic-NHp-CHn cyclic, m,n,p in (0,2)</t>
+  </si>
+  <si>
+    <t>Chm=Chn-F, m,n in (0,2)</t>
+  </si>
+  <si>
+    <t>AC-O-CHm</t>
+  </si>
+  <si>
+    <t>CHm cyclic-S-CHn cyclic, m,n in (0,2)</t>
+  </si>
+  <si>
+    <t>CHm=CHn—F, m,n in (0,2)</t>
+  </si>
+  <si>
+    <t>CHm=CHn—Br, m,n in (0,2)</t>
+  </si>
+  <si>
+    <t>CHm=CHn—I, m,n in (0,2)</t>
+  </si>
+  <si>
+    <t>ACBr</t>
+  </si>
+  <si>
+    <t>ACI</t>
+  </si>
+  <si>
+    <t>CHm(NH2)-COOH, m,n in (0,2)</t>
   </si>
 </sst>
 </file>
@@ -774,9 +774,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="303" zoomScaleNormal="303" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="DQ1" zoomScale="87" zoomScaleNormal="303" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:DR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -786,372 +786,372 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>33</v>
+      </c>
+      <c r="R1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S1" t="s">
+        <v>35</v>
+      </c>
+      <c r="T1" t="s">
+        <v>36</v>
+      </c>
+      <c r="U1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>63</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>66</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BI1" t="s">
+        <v>77</v>
+      </c>
+      <c r="BJ1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BK1" t="s">
+        <v>79</v>
+      </c>
+      <c r="BL1" t="s">
+        <v>80</v>
+      </c>
+      <c r="BM1" t="s">
+        <v>81</v>
+      </c>
+      <c r="BN1" t="s">
+        <v>82</v>
+      </c>
+      <c r="BO1" t="s">
+        <v>83</v>
+      </c>
+      <c r="BP1" t="s">
+        <v>84</v>
+      </c>
+      <c r="BQ1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BR1" t="s">
+        <v>86</v>
+      </c>
+      <c r="BS1" t="s">
+        <v>87</v>
+      </c>
+      <c r="BT1" t="s">
+        <v>88</v>
+      </c>
+      <c r="BU1" t="s">
+        <v>89</v>
+      </c>
+      <c r="BV1" t="s">
+        <v>90</v>
+      </c>
+      <c r="BW1" t="s">
+        <v>91</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY1" t="s">
+        <v>93</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CB1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="CC1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="CD1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="CE1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="CF1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="CG1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="CH1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="CI1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="CJ1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="CK1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="CL1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CM1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CO1" t="s">
+        <v>99</v>
+      </c>
+      <c r="CP1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="CQ1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>101</v>
+      </c>
+      <c r="CS1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="CT1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="CU1" t="s">
+        <v>102</v>
+      </c>
+      <c r="CV1" t="s">
+        <v>103</v>
+      </c>
+      <c r="CW1" t="s">
+        <v>104</v>
+      </c>
+      <c r="CX1" t="s">
+        <v>105</v>
+      </c>
+      <c r="CY1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="CZ1" t="s">
+        <v>106</v>
+      </c>
+      <c r="DA1" t="s">
+        <v>107</v>
+      </c>
+      <c r="DB1" t="s">
+        <v>108</v>
+      </c>
+      <c r="DC1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="DD1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>53</v>
-      </c>
-      <c r="BC1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BD1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BE1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BF1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BG1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>72</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>73</v>
-      </c>
-      <c r="BW1" t="s">
-        <v>74</v>
-      </c>
-      <c r="BX1" t="s">
-        <v>75</v>
-      </c>
-      <c r="BY1" t="s">
-        <v>76</v>
-      </c>
-      <c r="BZ1" t="s">
-        <v>77</v>
-      </c>
-      <c r="CA1" t="s">
-        <v>78</v>
-      </c>
-      <c r="CB1" t="s">
-        <v>79</v>
-      </c>
-      <c r="CC1" t="s">
-        <v>80</v>
-      </c>
-      <c r="CD1" t="s">
-        <v>81</v>
-      </c>
-      <c r="CE1" t="s">
-        <v>82</v>
-      </c>
-      <c r="CF1" t="s">
-        <v>83</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>84</v>
-      </c>
-      <c r="CH1" t="s">
-        <v>85</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>86</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CL1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CM1" t="s">
-        <v>90</v>
-      </c>
-      <c r="CN1" t="s">
-        <v>91</v>
-      </c>
-      <c r="CO1" t="s">
-        <v>92</v>
-      </c>
-      <c r="CP1" t="s">
-        <v>93</v>
-      </c>
-      <c r="CQ1" t="s">
-        <v>94</v>
-      </c>
-      <c r="CR1" t="s">
-        <v>95</v>
-      </c>
-      <c r="CS1" t="s">
-        <v>96</v>
-      </c>
-      <c r="CT1" t="s">
-        <v>97</v>
-      </c>
-      <c r="CU1" t="s">
-        <v>98</v>
-      </c>
-      <c r="CV1" t="s">
-        <v>99</v>
-      </c>
-      <c r="CW1" t="s">
-        <v>100</v>
-      </c>
-      <c r="CX1" t="s">
-        <v>101</v>
-      </c>
-      <c r="CY1" t="s">
-        <v>102</v>
-      </c>
-      <c r="CZ1" t="s">
-        <v>103</v>
-      </c>
-      <c r="DA1" t="s">
-        <v>104</v>
-      </c>
-      <c r="DB1" t="s">
-        <v>105</v>
-      </c>
-      <c r="DC1" t="s">
-        <v>106</v>
-      </c>
-      <c r="DD1" t="s">
-        <v>107</v>
-      </c>
       <c r="DE1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="DF1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="DG1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="DH1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="DI1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="DJ1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="DK1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="DL1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="DM1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="DN1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="DO1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="DP1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="DQ1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="DR1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:122" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>18</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1562,4 +1562,10 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{95965d95-ecc0-4720-b759-1f33c42ed7da}" enabled="1" method="Standard" siteId="{a0f29d7e-28cd-4f54-8442-7885aee7c080}" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>